<commit_message>
Many updates to the coil terminals
</commit_message>
<xml_diff>
--- a/SupportingDocs/Calculators/WDT.xlsx
+++ b/SupportingDocs/Calculators/WDT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\Coding\Masters\SupportingDocs\Calculators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38EBCB3C-5376-436F-B8CD-CB65ED62991B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0204CB3B-1977-4A48-808F-336C7212A2BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="2840" windowWidth="14400" windowHeight="7360" activeTab="2" xr2:uid="{6FE154D1-9408-484E-8BBE-1ECE0188AFD8}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="58">
   <si>
     <t>N</t>
   </si>
@@ -206,13 +206,19 @@
   </si>
   <si>
     <t>Anything + is lower</t>
+  </si>
+  <si>
+    <t>12s2pole,q=2</t>
+  </si>
+  <si>
+    <t>9s8pole,q=9/4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,6 +262,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -265,7 +279,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -282,11 +296,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -307,10 +330,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1295257-16CD-4001-9DF2-C6F519FD2D00}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -688,7 +715,7 @@
         <v>12</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -735,7 +762,7 @@
       </c>
       <c r="C9">
         <f>C6*C2/(2*C4*C10)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -747,7 +774,7 @@
       </c>
       <c r="C10">
         <f>GCD(C2,C5)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -771,7 +798,7 @@
       </c>
       <c r="C12">
         <f>(C2-C3)/(2*C5*C4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -795,7 +822,7 @@
       </c>
       <c r="C14">
         <f>C2/(C6*C5*C4)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -804,7 +831,7 @@
       </c>
       <c r="C15">
         <f>FLOOR(C12,1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -822,7 +849,7 @@
       </c>
       <c r="C17">
         <f>GCD(C16,C5)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -831,7 +858,7 @@
       </c>
       <c r="C18">
         <f>C2/C17</f>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -871,7 +898,7 @@
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="18" t="s">
         <v>51</v>
       </c>
       <c r="C22">
@@ -889,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1D9DA0-C87A-49C0-9BE1-89A4BDE34A77}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -950,7 +977,7 @@
         <v>12</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -997,7 +1024,7 @@
       </c>
       <c r="C9">
         <f>C6*C2/(2*C4*C10)</f>
-        <v>2.6666666666666665</v>
+        <v>5.333333333333333</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -1009,7 +1036,7 @@
       </c>
       <c r="C10">
         <f>GCD(C2,C5)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -1033,7 +1060,7 @@
       </c>
       <c r="C12">
         <f>(C2-C3)/(2*C5*C4)</f>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1045,7 +1072,7 @@
       </c>
       <c r="C13" t="b">
         <f>IF(MOD(C12,1)=0,TRUE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -1057,7 +1084,7 @@
       </c>
       <c r="C14">
         <f>C2/(C6*C5*C4)</f>
-        <v>1.3333333333333333</v>
+        <v>0.88888888888888884</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -1066,7 +1093,7 @@
       </c>
       <c r="C15">
         <f>FLOOR(C12,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1075,7 +1102,7 @@
       </c>
       <c r="C16">
         <f>C6*C5*(C12-C15)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1084,7 +1111,7 @@
       </c>
       <c r="C17">
         <f>GCD(C16,C5)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -1093,7 +1120,7 @@
       </c>
       <c r="C18">
         <f>C2/C17</f>
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -1102,7 +1129,7 @@
       </c>
       <c r="C19">
         <f>C5/C17</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -1136,10 +1163,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{867518C4-0CB7-4184-8BB9-867B8EA9A39B}">
-  <dimension ref="A1:Y43"/>
+  <dimension ref="A1:Y64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M55" sqref="M55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1161,10 +1188,10 @@
       <c r="C1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="18"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
@@ -1331,13 +1358,13 @@
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
@@ -1349,8 +1376,8 @@
       <c r="C8" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
@@ -1433,17 +1460,17 @@
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
@@ -1455,14 +1482,14 @@
       <c r="C16" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
@@ -1614,14 +1641,14 @@
       <c r="C23" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
@@ -1773,14 +1800,14 @@
       <c r="C30" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="18" t="s">
+      <c r="D30" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
@@ -1956,14 +1983,14 @@
       <c r="C37" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="18" t="s">
+      <c r="D37" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
@@ -2256,41 +2283,338 @@
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B43" s="18" t="s">
+      <c r="B43" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="18"/>
-      <c r="L43" s="18"/>
-      <c r="M43" s="18"/>
-      <c r="N43" s="18" t="s">
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="19"/>
+      <c r="M43" s="19"/>
+      <c r="N43" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="O43" s="18"/>
-      <c r="P43" s="18"/>
-      <c r="Q43" s="18"/>
-      <c r="R43" s="18"/>
-      <c r="S43" s="18"/>
+      <c r="O43" s="19"/>
+      <c r="P43" s="19"/>
+      <c r="Q43" s="19"/>
+      <c r="R43" s="19"/>
+      <c r="S43" s="19"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A45" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" t="s">
+        <v>38</v>
+      </c>
+      <c r="D46" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B47" s="20">
+        <v>1</v>
+      </c>
+      <c r="C47" s="20">
+        <v>2</v>
+      </c>
+      <c r="D47" s="20">
+        <v>3</v>
+      </c>
+      <c r="E47" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A48" s="20">
+        <v>1</v>
+      </c>
+      <c r="B48" s="3">
+        <v>1</v>
+      </c>
+      <c r="C48" s="21">
+        <v>2</v>
+      </c>
+      <c r="D48" s="8">
+        <v>3</v>
+      </c>
+      <c r="E48" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A49" s="20">
+        <v>2</v>
+      </c>
+      <c r="B49" s="9">
+        <v>5</v>
+      </c>
+      <c r="C49" s="22">
+        <v>6</v>
+      </c>
+      <c r="D49" s="3">
+        <v>7</v>
+      </c>
+      <c r="E49" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A50" s="20">
+        <v>3</v>
+      </c>
+      <c r="B50" s="8">
+        <v>9</v>
+      </c>
+      <c r="C50" s="23">
+        <v>10</v>
+      </c>
+      <c r="D50" s="9">
+        <v>11</v>
+      </c>
+      <c r="E50" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B53" t="s">
+        <v>38</v>
+      </c>
+      <c r="C53" t="s">
+        <v>38</v>
+      </c>
+      <c r="D53" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B54" s="20">
+        <v>1</v>
+      </c>
+      <c r="C54" s="20">
+        <v>2</v>
+      </c>
+      <c r="D54" s="20">
+        <v>3</v>
+      </c>
+      <c r="E54" s="20"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A55" s="20">
+        <v>1</v>
+      </c>
+      <c r="B55" s="3">
+        <v>1</v>
+      </c>
+      <c r="C55" s="21">
+        <v>8</v>
+      </c>
+      <c r="D55" s="8">
+        <v>6</v>
+      </c>
+      <c r="E55" s="8"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A56" s="20">
+        <v>2</v>
+      </c>
+      <c r="B56" s="9">
+        <v>4</v>
+      </c>
+      <c r="C56" s="22">
+        <v>2</v>
+      </c>
+      <c r="D56" s="3">
+        <v>4</v>
+      </c>
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57" s="20">
+        <v>3</v>
+      </c>
+      <c r="B57" s="8">
+        <v>7</v>
+      </c>
+      <c r="C57" s="23">
+        <v>5</v>
+      </c>
+      <c r="D57" s="9">
+        <v>3</v>
+      </c>
+      <c r="E57" s="9"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B60" t="s">
+        <v>38</v>
+      </c>
+      <c r="C60" t="s">
+        <v>38</v>
+      </c>
+      <c r="D60" t="s">
+        <v>38</v>
+      </c>
+      <c r="E60" t="s">
+        <v>38</v>
+      </c>
+      <c r="F60" t="s">
+        <v>38</v>
+      </c>
+      <c r="G60" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2">
+        <v>1</v>
+      </c>
+      <c r="C61" s="2">
+        <v>2</v>
+      </c>
+      <c r="D61" s="2">
+        <v>3</v>
+      </c>
+      <c r="E61" s="2">
+        <v>4</v>
+      </c>
+      <c r="F61" s="2">
+        <v>5</v>
+      </c>
+      <c r="G61" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A62" s="2">
+        <v>1</v>
+      </c>
+      <c r="B62" s="3">
+        <v>1</v>
+      </c>
+      <c r="C62" s="3">
+        <v>7</v>
+      </c>
+      <c r="D62" s="3">
+        <v>13</v>
+      </c>
+      <c r="E62" s="3">
+        <v>2</v>
+      </c>
+      <c r="F62" s="5">
+        <v>8</v>
+      </c>
+      <c r="G62" s="12">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A63" s="2">
+        <v>2</v>
+      </c>
+      <c r="B63" s="9">
+        <v>3</v>
+      </c>
+      <c r="C63" s="9">
+        <v>9</v>
+      </c>
+      <c r="D63" s="9">
+        <v>15</v>
+      </c>
+      <c r="E63" s="9">
+        <v>4</v>
+      </c>
+      <c r="F63" s="11">
+        <v>10</v>
+      </c>
+      <c r="G63" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A64" s="2">
+        <v>3</v>
+      </c>
+      <c r="B64" s="8">
+        <v>5</v>
+      </c>
+      <c r="C64" s="8">
+        <v>11</v>
+      </c>
+      <c r="D64" s="8">
+        <v>17</v>
+      </c>
+      <c r="E64" s="8">
+        <v>6</v>
+      </c>
+      <c r="F64" s="17">
+        <v>12</v>
+      </c>
+      <c r="G64" s="8">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="D45:I45"/>
+    <mergeCell ref="D52:I52"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D23:I23"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A15:I15"/>
     <mergeCell ref="D30:I30"/>
     <mergeCell ref="D37:I37"/>
     <mergeCell ref="B43:M43"/>
     <mergeCell ref="N43:S43"/>
     <mergeCell ref="D16:I16"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D23:I23"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A15:I15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>